<commit_message>
Use CELL("width") As Another Unimplemented Array Function
I might want to implement CHOOSECOLS after this PR is merged.
</commit_message>
<xml_diff>
--- a/tests/data/Reader/XLSX/atsign.choosecols.xlsx
+++ b/tests/data/Reader/XLSX/atsign.choosecols.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\atsign\tests\data\Reader\XLSX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{52B49DBE-5EB4-4438-9A8E-D6313AB31519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E18A5A-873A-4298-B28E-20AD07E3AD77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{AA1E5D37-8961-4234-8B6D-6F2A6C851B19}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -424,15 +424,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF22DA30-46A0-4500-9CE2-8038F13F2466}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>1</v>
       </c>
@@ -449,8 +449,16 @@
       <c r="G1">
         <v>1</v>
       </c>
+      <c r="I1" cm="1">
+        <f t="array" aca="1" ref="I1:J1" ca="1">CELL("width")</f>
+        <v>8</v>
+      </c>
+      <c r="J1" t="b">
+        <f ca="1"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2</v>
       </c>
@@ -467,7 +475,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>3</v>
       </c>
@@ -484,7 +492,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>4</v>
       </c>
@@ -501,7 +509,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>5</v>
       </c>

</xml_diff>